<commit_message>
uint unique ID support
</commit_message>
<xml_diff>
--- a/Assets/QuickSheet/Example/Excel/Example.xlsx
+++ b/Assets/QuickSheet/Example/Excel/Example.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Documents\Unity\QuickSheet\Assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\unity_quicksheet\Assets\QuickSheet\Example\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62649DB5-801A-410B-8034-867D99DBF764}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12682" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExcelExample" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>Id</t>
   </si>
@@ -75,18 +76,56 @@
   </si>
   <si>
     <t>Lurker</t>
+  </si>
+  <si>
+    <t>S001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S002</t>
+  </si>
+  <si>
+    <t>S003</t>
+  </si>
+  <si>
+    <t>S004</t>
+  </si>
+  <si>
+    <t>S005</t>
+  </si>
+  <si>
+    <t>S006</t>
+  </si>
+  <si>
+    <t>S007</t>
+  </si>
+  <si>
+    <t>S008</t>
+  </si>
+  <si>
+    <t>S009</t>
+  </si>
+  <si>
+    <t>S010</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -114,7 +153,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -130,7 +169,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -425,14 +464,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.95" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -449,8 +488,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
+      <c r="A2" t="s">
+        <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -463,8 +502,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
+      <c r="A3" t="s">
+        <v>18</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -477,8 +516,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
+      <c r="A4" t="s">
+        <v>19</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -491,8 +530,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
+      <c r="A5" t="s">
+        <v>20</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
@@ -505,8 +544,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
+      <c r="A6" t="s">
+        <v>21</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
@@ -519,8 +558,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
+      <c r="A7" t="s">
+        <v>22</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
@@ -533,8 +572,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
+      <c r="A8" t="s">
+        <v>23</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -547,8 +586,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
+      <c r="A9" t="s">
+        <v>24</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
@@ -561,8 +600,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>8</v>
+      <c r="A10" t="s">
+        <v>25</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -575,8 +614,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>9</v>
+      <c r="A11" t="s">
+        <v>26</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
@@ -589,6 +628,8 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
BitWise Support EnumType AutoGenerate
</commit_message>
<xml_diff>
--- a/Assets/QuickSheet/Example/Excel/Example.xlsx
+++ b/Assets/QuickSheet/Example/Excel/Example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\unity_quicksheet\Assets\QuickSheet\Example\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62649DB5-801A-410B-8034-867D99DBF764}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8230964-E2E5-4F49-8E78-3394AAD7CF81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="23452" windowHeight="12682" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,8 +24,70 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>KK47</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{D25225E7-9474-4E18-B0BD-DF1DFB7876E7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>枚举
+[Easy::1]
+[Medium::2]
+[Hard::3]</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{5EC8A9A7-CCB6-4C7D-A120-3852E15301B2}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">位组合
+[不可阻挡::1]
+[晕眩::2]
+[牛逼::3]
+[沉默::4]
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{32F215A2-36A1-4D4C-BCEC-3823942B8A91}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>枚举
+[Humanoid::1]
+[Monster::2]
+[Npc::3]</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
   <si>
     <t>Id</t>
   </si>
@@ -107,13 +169,53 @@
   </si>
   <si>
     <t>S010</t>
+  </si>
+  <si>
+    <t>Properties</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不可阻挡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>牛逼|沉默</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>晕眩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>晕眩|不可阻挡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>晕眩|da</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>晕眩|八八八</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Monster</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Humanoid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MonsterType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +229,19 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -464,16 +579,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.95" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -486,8 +604,14 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -500,8 +624,14 @@
       <c r="D2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -514,8 +644,14 @@
       <c r="D3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -528,8 +664,14 @@
       <c r="D4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -542,8 +684,14 @@
       <c r="D5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -556,8 +704,14 @@
       <c r="D6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -570,8 +724,14 @@
       <c r="D7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -584,8 +744,14 @@
       <c r="D8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -598,8 +764,14 @@
       <c r="D9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -612,8 +784,14 @@
       <c r="D10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -625,11 +803,18 @@
       </c>
       <c r="D11" t="s">
         <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>